<commit_message>
Diseño PCB de convertidor reductor de voltaje
</commit_message>
<xml_diff>
--- a/Tarea1/AUTOREVISION.xlsx
+++ b/Tarea1/AUTOREVISION.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F A Y M\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sistemas Embebidos II\IMT-322\Tarea1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3211F51B-8196-4D4D-B399-26C873C6370D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A064F6-F926-409F-AB96-13AD87FD5A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -223,7 +223,7 @@
     <t>SI</t>
   </si>
   <si>
-    <t>NO</t>
+    <t>Finalizado</t>
   </si>
 </sst>
 </file>
@@ -377,6 +377,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -389,10 +393,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,7 +733,7 @@
   <dimension ref="A1:F1032"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -747,46 +747,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="21" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -797,8 +797,8 @@
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="22" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -809,8 +809,8 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="22" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -821,10 +821,10 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -835,8 +835,8 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="22" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -847,8 +847,8 @@
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="22" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -859,8 +859,8 @@
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="22" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -871,8 +871,8 @@
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="22" t="s">
+      <c r="A11" s="22"/>
+      <c r="B11" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -883,8 +883,8 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="22" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -895,8 +895,8 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="22" t="s">
+      <c r="A13" s="22"/>
+      <c r="B13" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -907,8 +907,8 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="22" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -919,8 +919,8 @@
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="22" t="s">
+      <c r="A15" s="22"/>
+      <c r="B15" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -931,8 +931,8 @@
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="22" t="s">
+      <c r="A16" s="22"/>
+      <c r="B16" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -943,8 +943,8 @@
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="22" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -955,36 +955,36 @@
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="22" t="s">
+      <c r="A18" s="22"/>
+      <c r="B18" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="6"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="22" t="s">
+      <c r="A19" s="22"/>
+      <c r="B19" s="16" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="6"/>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="22" t="s">
+      <c r="A20" s="21"/>
+      <c r="B20" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="6"/>
@@ -994,7 +994,7 @@
       <c r="A21" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1005,10 +1005,10 @@
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1019,8 +1019,8 @@
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="22" t="s">
+      <c r="A23" s="22"/>
+      <c r="B23" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1031,8 +1031,8 @@
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="22" t="s">
+      <c r="A24" s="22"/>
+      <c r="B24" s="16" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1043,8 +1043,8 @@
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="22" t="s">
+      <c r="A25" s="21"/>
+      <c r="B25" s="16" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -1055,7 +1055,7 @@
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -1067,7 +1067,7 @@
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="6" t="s">
         <v>32</v>
       </c>
@@ -1077,7 +1077,7 @@
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="5" t="s">
         <v>33</v>
       </c>
@@ -1087,7 +1087,7 @@
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="5" t="s">
         <v>34</v>
       </c>
@@ -1097,7 +1097,7 @@
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="5" t="s">
         <v>35</v>
       </c>
@@ -1107,7 +1107,7 @@
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="5" t="s">
         <v>36</v>
       </c>
@@ -1117,7 +1117,7 @@
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="5" t="s">
         <v>37</v>
       </c>
@@ -1127,7 +1127,7 @@
       <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="5" t="s">
         <v>38</v>
       </c>
@@ -1137,7 +1137,7 @@
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="5" t="s">
         <v>39</v>
       </c>
@@ -1147,7 +1147,7 @@
       <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="5" t="s">
         <v>40</v>
       </c>
@@ -1157,7 +1157,7 @@
       <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="5" t="s">
         <v>41</v>
       </c>
@@ -1167,7 +1167,7 @@
       <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="5" t="s">
         <v>42</v>
       </c>
@@ -1177,7 +1177,7 @@
       <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="20"/>
+      <c r="A38" s="22"/>
       <c r="B38" s="5" t="s">
         <v>43</v>
       </c>
@@ -1187,7 +1187,7 @@
       <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
+      <c r="A39" s="22"/>
       <c r="B39" s="5" t="s">
         <v>44</v>
       </c>
@@ -1197,7 +1197,7 @@
       <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="20"/>
+      <c r="A40" s="22"/>
       <c r="B40" s="5" t="s">
         <v>45</v>
       </c>
@@ -1207,7 +1207,7 @@
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A41" s="20"/>
+      <c r="A41" s="22"/>
       <c r="B41" s="5" t="s">
         <v>46</v>
       </c>
@@ -1217,7 +1217,7 @@
       <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A42" s="20"/>
+      <c r="A42" s="22"/>
       <c r="B42" s="5" t="s">
         <v>47</v>
       </c>
@@ -1227,7 +1227,7 @@
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="6" t="s">
         <v>48</v>
       </c>
@@ -1237,7 +1237,7 @@
       <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
+      <c r="A44" s="22"/>
       <c r="B44" s="6" t="s">
         <v>49</v>
       </c>
@@ -1247,7 +1247,7 @@
       <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="6" t="s">
         <v>50</v>
       </c>
@@ -1257,7 +1257,7 @@
       <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
+      <c r="A46" s="22"/>
       <c r="B46" s="5" t="s">
         <v>51</v>
       </c>
@@ -1267,7 +1267,7 @@
       <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="5" t="s">
         <v>52</v>
       </c>
@@ -1277,7 +1277,7 @@
       <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="5"/>
       <c r="C48" s="7"/>
       <c r="D48" s="6"/>
@@ -1285,7 +1285,7 @@
       <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
+      <c r="A49" s="22"/>
       <c r="B49" s="5" t="s">
         <v>53</v>
       </c>
@@ -1295,7 +1295,7 @@
       <c r="F49" s="4"/>
     </row>
     <row r="50" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
+      <c r="A50" s="22"/>
       <c r="B50" s="5" t="s">
         <v>54</v>
       </c>
@@ -1305,7 +1305,7 @@
       <c r="F50" s="4"/>
     </row>
     <row r="51" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
+      <c r="A51" s="22"/>
       <c r="B51" s="5" t="s">
         <v>55</v>
       </c>
@@ -1315,7 +1315,7 @@
       <c r="F51" s="4"/>
     </row>
     <row r="52" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
+      <c r="A52" s="22"/>
       <c r="B52" s="5"/>
       <c r="C52" s="7"/>
       <c r="D52" s="6"/>
@@ -1323,7 +1323,7 @@
       <c r="F52" s="4"/>
     </row>
     <row r="53" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A53" s="20"/>
+      <c r="A53" s="22"/>
       <c r="B53" s="5" t="s">
         <v>56</v>
       </c>
@@ -1333,7 +1333,7 @@
       <c r="F53" s="4"/>
     </row>
     <row r="54" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
+      <c r="A54" s="22"/>
       <c r="B54" s="5" t="s">
         <v>57</v>
       </c>
@@ -1343,7 +1343,7 @@
       <c r="F54" s="4"/>
     </row>
     <row r="55" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A55" s="20"/>
+      <c r="A55" s="22"/>
       <c r="B55" s="5" t="s">
         <v>58</v>
       </c>
@@ -1353,7 +1353,7 @@
       <c r="F55" s="4"/>
     </row>
     <row r="56" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A56" s="20"/>
+      <c r="A56" s="22"/>
       <c r="B56" s="5" t="s">
         <v>59</v>
       </c>
@@ -1363,7 +1363,7 @@
       <c r="F56" s="4"/>
     </row>
     <row r="57" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A57" s="20"/>
+      <c r="A57" s="22"/>
       <c r="B57" s="5" t="s">
         <v>60</v>
       </c>
@@ -1373,7 +1373,7 @@
       <c r="F57" s="4"/>
     </row>
     <row r="58" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A58" s="20"/>
+      <c r="A58" s="22"/>
       <c r="B58" s="5" t="s">
         <v>61</v>
       </c>
@@ -1383,7 +1383,7 @@
       <c r="F58" s="4"/>
     </row>
     <row r="59" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A59" s="20"/>
+      <c r="A59" s="22"/>
       <c r="B59" s="5" t="s">
         <v>62</v>
       </c>
@@ -1395,7 +1395,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A60" s="20"/>
+      <c r="A60" s="22"/>
       <c r="B60" s="5" t="s">
         <v>64</v>
       </c>
@@ -1405,7 +1405,7 @@
       <c r="F60" s="4"/>
     </row>
     <row r="61" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A61" s="19"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="5" t="s">
         <v>65</v>
       </c>
@@ -1418,7 +1418,7 @@
       <c r="A62" s="11"/>
     </row>
     <row r="76" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A76" s="17"/>
+      <c r="A76" s="19"/>
       <c r="B76" s="12"/>
       <c r="C76" s="13"/>
       <c r="D76" s="13"/>
@@ -1426,7 +1426,7 @@
       <c r="F76" s="13"/>
     </row>
     <row r="77" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A77" s="16"/>
+      <c r="A77" s="18"/>
       <c r="B77" s="12"/>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
@@ -1434,7 +1434,7 @@
       <c r="F77" s="13"/>
     </row>
     <row r="78" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A78" s="16"/>
+      <c r="A78" s="18"/>
       <c r="B78" s="12"/>
       <c r="C78" s="13"/>
       <c r="D78" s="13"/>
@@ -1442,7 +1442,7 @@
       <c r="F78" s="13"/>
     </row>
     <row r="79" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A79" s="16"/>
+      <c r="A79" s="18"/>
       <c r="B79" s="12"/>
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
@@ -1450,7 +1450,7 @@
       <c r="F79" s="13"/>
     </row>
     <row r="80" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A80" s="16"/>
+      <c r="A80" s="18"/>
       <c r="B80" s="13"/>
       <c r="C80" s="13"/>
       <c r="D80" s="13"/>

</xml_diff>